<commit_message>
feat: update Project interface with additional properties
</commit_message>
<xml_diff>
--- a/public/mock-projects.xlsx
+++ b/public/mock-projects.xlsx
@@ -1,25 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27624"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{04CB3999-E5C7-4415-AC69-C12756222018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>id</t>
   </si>
@@ -42,6 +54,12 @@
     <t>images</t>
   </si>
   <si>
+    <t>slug</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
     <t>Proyecto Uno</t>
   </si>
   <si>
@@ -49,13 +67,22 @@
   </si>
   <si>
     <t>Blvd. Juan Bautista Escalante</t>
+  </si>
+  <si>
+    <t>project-1-first.png,project-1-second.png,project-1-third.png,project-1-fourth.jpg,project-1-fifth.jpg,project-1-six.jpg</t>
+  </si>
+  <si>
+    <t>project-one</t>
+  </si>
+  <si>
+    <t>Cillum consectetur fugiat consequat cillum consequat exercitation qui dolore eu quis proident culpa duis. Exercitation exercitation non esse officia proident ipsum cupidatat nulla duis mollit laborum nostrud. Commodo enim exercitation veniam nisi ipsum ut laborum consectetur. Dolor  Dolor labore Lorem id cupidatat ea commodo incididunt incididunt elit ipsum labore Lorem veniam laboris. Amet adipisicing voluptate nostrud amet laborum sunt sint nulla est elit est dolor cupidatat nostrud. Velit aliqua fugiat enim aliqua cillum reprehenderit. Lorem adipisicing enim consectetur qui voluptate est eu nostrud cillum magna proident et in. Est elit culpa et anim consectetur dolore magna non incididunt veniam pariatur. Ut duis reprehenderit est aliquip eiusmod aliquip do magna esse ex. Minim proident enim Lorem dolor. Dolor labore Lorem id cupidatat ea commodo incididunt incididunt elit ipsum labore Lorem veniam laboris. Amet adipisicing voluptate nostrud amet laborum sunt sint nulla est elit est dolor cupidatat nostrud. Velit aliqua fugiat enim aliqua cillum reprehenderit. Lorem adipisicing enim consectetur qui voluptate est eu nostrud cillum magna proident et in. Est elit culpa et anim consectetur dolore magna non incididunt veniam pariatur. Ut duis reprehenderit est aliquip eiusmod aliquip do magna esse ex. Minim proident enim Lorem dolor.amet do velit nisi deserunt aliquip consequat. Minim aliquip dolore irure sint labore sunt incididunt qui nostrud.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -365,21 +392,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
   <cols>
-    <col min="2" max="2" width="23.33203125" customWidth="1"/>
-    <col min="3" max="3" width="48.77734375" customWidth="1"/>
-    <col min="4" max="4" width="28.21875" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+    <col min="3" max="3" width="48.7109375" customWidth="1"/>
+    <col min="4" max="4" width="28.28515625" customWidth="1"/>
+    <col min="7" max="7" width="35.85546875" customWidth="1"/>
+    <col min="8" max="8" width="16" customWidth="1"/>
+    <col min="9" max="9" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -401,25 +431,40 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="15">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E2">
         <v>29.146880118507202</v>
       </c>
       <c r="F2">
         <v>-110.95623684623</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>